<commit_message>
Atualização depois da Sprint 2A
</commit_message>
<xml_diff>
--- a/Documentação/PlanoDeAção_BeCold.xlsx
+++ b/Documentação/PlanoDeAção_BeCold.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3FD0ED8-20FF-49A3-9AEE-2BE3A17777B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E40B2A1-8EDF-4534-8072-929C6A2A3C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do plano de Ação" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>Dados do plano de marketing</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Não Iniciado</t>
-  </si>
-  <si>
-    <t>Em Andamento</t>
   </si>
   <si>
     <t>Atrasado</t>
@@ -172,6 +169,12 @@
   </si>
   <si>
     <t>Placeholder</t>
+  </si>
+  <si>
+    <t>Script Banco de Dados</t>
+  </si>
+  <si>
+    <t>Próxima Semana</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +626,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE29908"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -954,7 +963,7 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1006,20 +1015,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="16" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="16" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="15" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1030,14 +1027,29 @@
     <xf numFmtId="0" fontId="15" fillId="13" borderId="16" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="16" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="16" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -1094,7 +1106,7 @@
     <cellStyle name="Total" xfId="35" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vírgula" xfId="20" builtinId="3" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="43">
     <dxf>
       <font>
         <b/>
@@ -1338,6 +1350,102 @@
         <i val="0"/>
         <color theme="1"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
       <border>
         <top style="thin">
           <color theme="1" tint="0.34998626667073579"/>
@@ -1455,16 +1563,21 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Plano de marketing" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Lista de planos" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="34"/>
-      <tableStyleElement type="headerRow" dxfId="33"/>
-      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="wholeTable" dxfId="42"/>
+      <tableStyleElement type="headerRow" dxfId="41"/>
+      <tableStyleElement type="firstRowStripe" dxfId="40"/>
     </tableStyle>
     <tableStyle name="Plano de marketing" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="31"/>
-      <tableStyleElement type="headerRow" dxfId="30"/>
-      <tableStyleElement type="totalRow" dxfId="29"/>
+      <tableStyleElement type="wholeTable" dxfId="39"/>
+      <tableStyleElement type="headerRow" dxfId="38"/>
+      <tableStyleElement type="totalRow" dxfId="37"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFE29908"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6166,8 +6279,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Dados" displayName="Dados" ref="B6:G18" headerRowDxfId="28">
-  <autoFilter ref="B6:G18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Dados" displayName="Dados" ref="B6:G19" headerRowDxfId="28">
+  <autoFilter ref="B6:G19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa" totalsRowLabel="Total" dataDxfId="27"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Status" totalsRowFunction="count" dataDxfId="26"/>
@@ -6531,10 +6644,10 @@
     <tabColor theme="4" tint="0.39997558519241921"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G18"/>
+  <dimension ref="B1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6547,55 +6660,59 @@
   <sheetData>
     <row r="1" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="9"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="21"/>
-      <c r="C2" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="21"/>
+      <c r="B2"/>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
+      <c r="G2"/>
     </row>
     <row r="3" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="23" t="s">
+      <c r="D3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3"/>
+      <c r="G3" s="27" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4"/>
+        <v>7</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5"/>
@@ -6613,30 +6730,30 @@
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,25)</f>
@@ -6649,38 +6766,38 @@
     </row>
     <row r="8" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,26)</f>
         <v>45195</v>
       </c>
-      <c r="G8" s="14" t="e">
-        <f ca="1">DATE(YEAR(TODAY())*0,0,0)</f>
-        <v>#NUM!</v>
+      <c r="G8" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,29)</f>
+        <v>45198</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,28)</f>
@@ -6693,43 +6810,47 @@
     </row>
     <row r="10" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="14" t="e">
-        <f t="shared" ref="F9:G18" ca="1" si="0">DATE(YEAR(TODAY())*0,0,0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G10" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
+      <c r="F10" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
+      </c>
+      <c r="G10" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="E11" s="13"/>
-      <c r="F11" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="G11" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
+      <c r="F11" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
+      </c>
+      <c r="G11" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>3</v>
@@ -6737,7 +6858,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="F10:G19" ca="1" si="0">DATE(YEAR(TODAY())*0,0,0)</f>
         <v>#NUM!</v>
       </c>
       <c r="G12" s="14" t="e">
@@ -6747,7 +6868,7 @@
     </row>
     <row r="13" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>3</v>
@@ -6765,7 +6886,7 @@
     </row>
     <row r="14" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>3</v>
@@ -6783,7 +6904,7 @@
     </row>
     <row r="15" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>3</v>
@@ -6801,7 +6922,7 @@
     </row>
     <row r="16" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>3</v>
@@ -6819,7 +6940,7 @@
     </row>
     <row r="17" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>3</v>
@@ -6837,7 +6958,7 @@
     </row>
     <row r="18" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>3</v>
@@ -6851,6 +6972,26 @@
       <c r="G18" s="14" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
+      </c>
+      <c r="G19" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
       </c>
     </row>
   </sheetData>
@@ -6858,39 +6999,67 @@
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="C2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:G18">
-    <cfRule type="expression" dxfId="15" priority="15">
+  <conditionalFormatting sqref="B7:G19">
+    <cfRule type="expression" dxfId="36" priority="23">
       <formula>(clPersonalizado2="ATIVADO")*($C7=txtPersonalizado2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="35" priority="24">
       <formula>(clPersonalizado3="ATIVADO")*($C7=txtPersonalizado3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="17">
+    <cfRule type="expression" dxfId="34" priority="25">
       <formula>(clPersonalizado4="ATIVADO")*($C7=txtPersonalizado4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:G18">
-    <cfRule type="expression" dxfId="12" priority="1">
+  <conditionalFormatting sqref="B7:G19">
+    <cfRule type="expression" dxfId="33" priority="9">
       <formula>($C7="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="32" priority="13">
       <formula>($C7="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="31" priority="14">
       <formula>($C7="Atrasado")*(clAtrasado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="30" priority="20">
       <formula>($C7="Concluído")*(clConcluído="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="14">
+    <cfRule type="expression" dxfId="29" priority="22">
       <formula>(clPersonalizado1="ATIVADO")*($C7=txtPersonalizado1)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B19:G19">
+    <cfRule type="expression" dxfId="15" priority="6">
+      <formula>(clPersonalizado2="ATIVADO")*($C19=txtPersonalizado2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="7">
+      <formula>(clPersonalizado3="ATIVADO")*($C19=txtPersonalizado3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="8">
+      <formula>(clPersonalizado4="ATIVADO")*($C19=txtPersonalizado4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:G19">
+    <cfRule type="expression" dxfId="12" priority="1">
+      <formula>($C19="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="2">
+      <formula>($C19="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>($C19="Atrasado")*(clAtrasado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>($C19="Concluído")*(clConcluído="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="5">
+      <formula>(clPersonalizado1="ATIVADO")*($C19=txtPersonalizado1)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations xWindow="1742" yWindow="648" count="17">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Ativado ou Desativado. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" prompt="Selecione Ativado ou Desativado nesta célula para alternar o destaque da linha para o status acima. Pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C4:F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Ativado ou Desativado. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" prompt="Selecione Ativado ou Desativado nesta célula para alternar o destaque da linha para o status acima. Pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C4:G4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"ATIVADO,DESATIVADO"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Atribuído a na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="E7:E18" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Atribuído a na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="E7:E19" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Nomes</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Crie um plano de projeto de Marketing nesta pasta de trabalho. Organize os dados e insira os detalhes na tabela Dados nesta planilha iniciando na célula B6. Selecione a célula B2 para navegar para a planilha Dados da lista" sqref="A1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
@@ -6904,12 +7073,12 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Não iniciado está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="C3" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Em Andamento está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="D3" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Atrasado está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="E3" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Concluído está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="F3" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Concluído está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="F3:G3" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="O título desta planilha está nesta célula. Selecione a célula abaixo para navegar até a planilha Dados da lista. As categorias de status estão nas células D3 a K4" sqref="B1" xr:uid="{00000000-0002-0000-0000-000015000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Nome do proprietário na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="D7:D18" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Nome do proprietário na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="D7:D19" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>Nomes</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Status na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C7:C18" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Status na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C7:C19" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$C$3:$F$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -6935,7 +7104,7 @@
   <dimension ref="B1:C12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6947,83 +7116,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="18"/>
+      <c r="B1" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="25"/>
     </row>
     <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="11"/>
-      <c r="C3" s="19" t="s">
-        <v>30</v>
+      <c r="C3" s="17" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:3" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7058,6 +7227,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf6cf056b5324d160236e2ac13572175">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="308e4927137fd5e63b6be1bd7725299e" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7277,25 +7464,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB26FF4A-9A24-42D8-B946-9CA436224F6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99945BEB-7D41-4FB6-9D32-A35A84B455C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ACF481C-B850-47D3-8383-E0C13159DD26}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7313,22 +7500,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99945BEB-7D41-4FB6-9D32-A35A84B455C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB26FF4A-9A24-42D8-B946-9CA436224F6C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adicionado a semana nas tarefas do plano de ação
</commit_message>
<xml_diff>
--- a/Documentação/PlanoDeAção_BeCold.xlsx
+++ b/Documentação/PlanoDeAção_BeCold.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E40B2A1-8EDF-4534-8072-929C6A2A3C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE09DEF3-D167-453E-8038-677EA57A83D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do plano de Ação" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>Dados do plano de marketing</t>
   </si>
@@ -174,7 +174,13 @@
     <t>Script Banco de Dados</t>
   </si>
   <si>
-    <t>Próxima Semana</t>
+    <t>Semana</t>
+  </si>
+  <si>
+    <t>Semana 2-A</t>
+  </si>
+  <si>
+    <t>Semana 2-B</t>
   </si>
 </sst>
 </file>
@@ -418,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -626,12 +632,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE29908"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -963,7 +963,7 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1045,11 +1045,8 @@
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="16" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -1106,66 +1103,9 @@
     <cellStyle name="Total" xfId="35" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vírgula" xfId="20" builtinId="3" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="36">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1265,6 +1205,34 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <color theme="5" tint="-0.499984740745262"/>
@@ -1298,51 +1266,6 @@
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1405,40 +1328,37 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <color theme="7" tint="-0.499984740745262"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1563,14 +1483,14 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Plano de marketing" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Lista de planos" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="42"/>
-      <tableStyleElement type="headerRow" dxfId="41"/>
-      <tableStyleElement type="firstRowStripe" dxfId="40"/>
+      <tableStyleElement type="wholeTable" dxfId="35"/>
+      <tableStyleElement type="headerRow" dxfId="34"/>
+      <tableStyleElement type="firstRowStripe" dxfId="33"/>
     </tableStyle>
     <tableStyle name="Plano de marketing" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="39"/>
-      <tableStyleElement type="headerRow" dxfId="38"/>
-      <tableStyleElement type="totalRow" dxfId="37"/>
+      <tableStyleElement type="wholeTable" dxfId="32"/>
+      <tableStyleElement type="headerRow" dxfId="31"/>
+      <tableStyleElement type="totalRow" dxfId="30"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -6279,15 +6199,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Dados" displayName="Dados" ref="B6:G19" headerRowDxfId="28">
-  <autoFilter ref="B6:G19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa" totalsRowLabel="Total" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Status" totalsRowFunction="count" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Responsável" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Atribuído a" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Data de início" dataDxfId="23" dataCellStyle="Data"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Data de término" dataDxfId="22" dataCellStyle="Data"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Dados" displayName="Dados" ref="B6:H19" headerRowDxfId="29">
+  <autoFilter ref="B6:H19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa" totalsRowLabel="Total" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Status" totalsRowFunction="count" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Semana" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Responsável" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Atribuído a" dataDxfId="11" dataCellStyle="Data"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Data de início" dataDxfId="10" dataCellStyle="Data"/>
+    <tableColumn id="6" xr3:uid="{B3EC7629-E4DA-4FA6-BCF2-5E4DC4390764}" name="Data de término" dataDxfId="9" dataCellStyle="Data"/>
   </tableColumns>
   <tableStyleInfo name="Plano de marketing" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -6299,11 +6220,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Pessoas" displayName="Pessoas" ref="B4:C11" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Pessoas" displayName="Pessoas" ref="B4:C11" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="B4:C11" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Nome" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cargo" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Nome" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cargo" totalsRowFunction="count" dataDxfId="22" totalsRowDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="Lista de planos" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -6644,10 +6565,10 @@
     <tabColor theme="4" tint="0.39997558519241921"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G19"/>
+  <dimension ref="B1:H19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6655,10 +6576,10 @@
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="64.25" style="1" customWidth="1"/>
     <col min="3" max="7" width="17.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="2.5" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
@@ -6668,7 +6589,7 @@
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
     </row>
-    <row r="2" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2"/>
       <c r="C2" s="22" t="s">
         <v>6</v>
@@ -6678,7 +6599,7 @@
       <c r="F2" s="24"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -6692,11 +6613,9 @@
       <c r="F3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="27" t="s">
-        <v>41</v>
-      </c>
+      <c r="G3"/>
     </row>
-    <row r="4" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
         <v>7</v>
@@ -6710,11 +6629,9 @@
       <c r="F4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>7</v>
-      </c>
+      <c r="G4"/>
     </row>
-    <row r="5" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
@@ -6722,7 +6639,7 @@
       <c r="F5"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
         <v>1</v>
       </c>
@@ -6730,19 +6647,22 @@
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="F6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="G6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="H6" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>24</v>
       </c>
@@ -6750,21 +6670,24 @@
         <v>5</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="14">
+      <c r="G7" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,25)</f>
         <v>45194</v>
       </c>
-      <c r="G7" s="14">
+      <c r="H7" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,27)</f>
         <v>45196</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>27</v>
       </c>
@@ -6772,21 +6695,24 @@
         <v>5</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="14">
+      <c r="G8" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,26)</f>
         <v>45195</v>
       </c>
-      <c r="G8" s="14">
+      <c r="H8" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,29)</f>
         <v>45198</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>28</v>
       </c>
@@ -6794,21 +6720,24 @@
         <v>5</v>
       </c>
       <c r="D9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="14">
+      <c r="G9" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,28)</f>
         <v>45197</v>
       </c>
-      <c r="G9" s="14">
+      <c r="H9" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,29)</f>
         <v>45198</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>30</v>
       </c>
@@ -6816,19 +6745,22 @@
         <v>3</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14">
+      <c r="F10" s="27"/>
+      <c r="G10" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
         <v>45171</v>
       </c>
-      <c r="G10" s="14">
+      <c r="H10" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
         <v>45175</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>31</v>
       </c>
@@ -6836,145 +6768,169 @@
         <v>3</v>
       </c>
       <c r="D11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14">
+      <c r="F11" s="27"/>
+      <c r="G11" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
         <v>45171</v>
       </c>
-      <c r="G11" s="14">
+      <c r="H11" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
         <v>45175</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="14" t="e">
-        <f t="shared" ref="F10:G19" ca="1" si="0">DATE(YEAR(TODAY())*0,0,0)</f>
+      <c r="F12" s="27"/>
+      <c r="G12" s="14" t="e">
+        <f t="shared" ref="G12:H18" ca="1" si="0">DATE(YEAR(TODAY())*0,0,0)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G12" s="14" t="e">
+      <c r="H12" s="14" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
+      <c r="F13" s="27"/>
       <c r="G13" s="14" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#NUM!</v>
       </c>
+      <c r="H13" s="14" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="14" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E14" s="13"/>
-      <c r="F14" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
+      <c r="F14" s="27"/>
       <c r="G14" s="14" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#NUM!</v>
       </c>
+      <c r="H14" s="14" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="15" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
+      <c r="F15" s="27"/>
       <c r="G15" s="14" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#NUM!</v>
       </c>
+      <c r="H15" s="14" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="16" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
+      <c r="F16" s="27"/>
       <c r="G16" s="14" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#NUM!</v>
       </c>
+      <c r="H16" s="14" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="17" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E17" s="13"/>
-      <c r="F17" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
+      <c r="F17" s="27"/>
       <c r="G17" s="14" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#NUM!</v>
       </c>
+      <c r="H17" s="14" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="18" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E18" s="13"/>
-      <c r="F18" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
+      <c r="F18" s="27"/>
       <c r="G18" s="14" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#NUM!</v>
       </c>
+      <c r="H18" s="14" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
         <v>40</v>
       </c>
@@ -6982,14 +6938,17 @@
         <v>3</v>
       </c>
       <c r="D19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14">
+      <c r="F19" s="27"/>
+      <c r="G19" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
         <v>45171</v>
       </c>
-      <c r="G19" s="14">
+      <c r="H19" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
         <v>45175</v>
       </c>
@@ -6999,83 +6958,79 @@
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="C2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:G19">
-    <cfRule type="expression" dxfId="36" priority="23">
+  <conditionalFormatting sqref="E7:H19 B7:C19">
+    <cfRule type="expression" dxfId="20" priority="17">
+      <formula>($C7="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>($C7="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>($C7="Atrasado")*(clAtrasado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="28">
+      <formula>($C7="Concluído")*(clConcluído="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="30">
+      <formula>(clPersonalizado1="ATIVADO")*($C7=txtPersonalizado1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="31">
       <formula>(clPersonalizado2="ATIVADO")*($C7=txtPersonalizado2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="24">
+    <cfRule type="expression" dxfId="14" priority="32">
       <formula>(clPersonalizado3="ATIVADO")*($C7=txtPersonalizado3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="25">
+    <cfRule type="expression" dxfId="13" priority="33">
       <formula>(clPersonalizado4="ATIVADO")*($C7=txtPersonalizado4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:G19">
-    <cfRule type="expression" dxfId="33" priority="9">
+  <conditionalFormatting sqref="D7:D19">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>($C7="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="13">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>($C7="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="14">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>($C7="Atrasado")*(clAtrasado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="20">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>($C7="Concluído")*(clConcluído="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="22">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>(clPersonalizado1="ATIVADO")*($C7=txtPersonalizado1)</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:G19">
-    <cfRule type="expression" dxfId="15" priority="6">
-      <formula>(clPersonalizado2="ATIVADO")*($C19=txtPersonalizado2)</formula>
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>(clPersonalizado2="ATIVADO")*($C7=txtPersonalizado2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="7">
-      <formula>(clPersonalizado3="ATIVADO")*($C19=txtPersonalizado3)</formula>
+    <cfRule type="expression" dxfId="2" priority="7">
+      <formula>(clPersonalizado3="ATIVADO")*($C7=txtPersonalizado3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="8">
-      <formula>(clPersonalizado4="ATIVADO")*($C19=txtPersonalizado4)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:G19">
-    <cfRule type="expression" dxfId="12" priority="1">
-      <formula>($C19="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
-      <formula>($C19="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="3">
-      <formula>($C19="Atrasado")*(clAtrasado="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4">
-      <formula>($C19="Concluído")*(clConcluído="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="5">
-      <formula>(clPersonalizado1="ATIVADO")*($C19=txtPersonalizado1)</formula>
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>(clPersonalizado4="ATIVADO")*($C7=txtPersonalizado4)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="1742" yWindow="648" count="17">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Ativado ou Desativado. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" prompt="Selecione Ativado ou Desativado nesta célula para alternar o destaque da linha para o status acima. Pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C4:G4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Ativado ou Desativado. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" prompt="Selecione Ativado ou Desativado nesta célula para alternar o destaque da linha para o status acima. Pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C4:F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"ATIVADO,DESATIVADO"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Atribuído a na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="E7:E19" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Atribuído a na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="F7:F19" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Nomes</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Crie um plano de projeto de Marketing nesta pasta de trabalho. Organize os dados e insira os detalhes na tabela Dados nesta planilha iniciando na célula B6. Selecione a célula B2 para navegar para a planilha Dados da lista" sqref="A1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="As categorias de status são definidas nas células D3 até K4.. Personalize as categorias de Status para corresponder aos dados de plano de marketing. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha" sqref="D1:G1" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a Tarefa na coluna sob este cabeçalho. Use os filtros de cabeçalho para localizar itens específicos" sqref="B6" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Selecione Status nesta coluna nesse cabeçalho. Pressione Alt+Seta para baixo para abrir a lista suspensa, em seguida, pressione Enter para fazer a seleção" sqref="C6" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Selecione Proprietário nesta coluna nesse cabeçalho. Pressione Alt+Seta para baixo para abrir a lista suspensa, em seguida, pressione Enter para fazer a seleção" sqref="D6" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Selecione Atribuído a nome da pessoa nesta coluna nesse cabeçalho. Pressione Alt+Seta para baixo para abrir a lista suspensa, em seguida, pressione Enter para fazer a seleção" sqref="E6" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a Data de início antecipado na coluna sob este cabeçalho" sqref="F6" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a Data de término antecipado na coluna sob este cabeçalho" sqref="G6" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Selecione Proprietário nesta coluna nesse cabeçalho. Pressione Alt+Seta para baixo para abrir a lista suspensa, em seguida, pressione Enter para fazer a seleção" sqref="E6" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Selecione Atribuído a nome da pessoa nesta coluna nesse cabeçalho. Pressione Alt+Seta para baixo para abrir a lista suspensa, em seguida, pressione Enter para fazer a seleção" sqref="F6" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a Data de início antecipado na coluna sob este cabeçalho" sqref="G6" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a Data de término antecipado na coluna sob este cabeçalho" sqref="H6" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Não iniciado está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="C3" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Em Andamento está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="D3" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Atrasado está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="E3" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Concluído está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="F3:G3" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Concluído está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="F3" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="O título desta planilha está nesta célula. Selecione a célula abaixo para navegar até a planilha Dados da lista. As categorias de status estão nas células D3 a K4" sqref="B1" xr:uid="{00000000-0002-0000-0000-000015000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Nome do proprietário na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="D7:D19" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Nome do proprietário na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="E7:E19" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>Nomes</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Status na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C7:C19" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -7227,24 +7182,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf6cf056b5324d160236e2ac13572175">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="308e4927137fd5e63b6be1bd7725299e" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7464,25 +7401,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB26FF4A-9A24-42D8-B946-9CA436224F6C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99945BEB-7D41-4FB6-9D32-A35A84B455C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ACF481C-B850-47D3-8383-E0C13159DD26}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7500,4 +7437,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99945BEB-7D41-4FB6-9D32-A35A84B455C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB26FF4A-9A24-42D8-B946-9CA436224F6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Peso das Atividades Yuri | Atas das daily da semana
</commit_message>
<xml_diff>
--- a/Documentação/PlanoDeAção_BeCold.xlsx
+++ b/Documentação/PlanoDeAção_BeCold.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE09DEF3-D167-453E-8038-677EA57A83D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839B067E-B51D-49BA-AC80-D655DE1EADAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
   <si>
     <t>Dados do plano de marketing</t>
   </si>
@@ -123,18 +123,6 @@
     <t>Developer</t>
   </si>
   <si>
-    <t>Análise de Entregaveis Sprint 1</t>
-  </si>
-  <si>
-    <t>Data de início</t>
-  </si>
-  <si>
-    <t>Data de término</t>
-  </si>
-  <si>
-    <t>Documentação Segunda Versão</t>
-  </si>
-  <si>
     <t>Modelagem Banco de Dados Primeira Versão</t>
   </si>
   <si>
@@ -159,9 +147,6 @@
     <t>Página Dashboard Estática</t>
   </si>
   <si>
-    <t>Integração Captura de Dados com ChartJs</t>
-  </si>
-  <si>
     <t>Diagrama de solução</t>
   </si>
   <si>
@@ -181,6 +166,39 @@
   </si>
   <si>
     <t>Semana 2-B</t>
+  </si>
+  <si>
+    <t>Documentação Atualizada</t>
+  </si>
+  <si>
+    <t>Atualização GitHub do Projeto</t>
+  </si>
+  <si>
+    <t>Planilha de Riscos do Projeto</t>
+  </si>
+  <si>
+    <t>Teste com Sensor do Projeto + Gráficos</t>
+  </si>
+  <si>
+    <t>Atividades organizadas na ferramenta de Gestão (Sprints / Atividades)</t>
+  </si>
+  <si>
+    <t>Semana 2-C</t>
+  </si>
+  <si>
+    <t>Semana 2-D</t>
+  </si>
+  <si>
+    <t>Ester, Kaiqui e Paulo</t>
+  </si>
+  <si>
+    <t>Thalita e Yuri</t>
+  </si>
+  <si>
+    <t>Previsão de início</t>
+  </si>
+  <si>
+    <t>Previsão de término</t>
   </si>
 </sst>
 </file>
@@ -1027,6 +1045,9 @@
     <xf numFmtId="0" fontId="15" fillId="13" borderId="16" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1044,9 +1065,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -1103,9 +1121,186 @@
     <cellStyle name="Total" xfId="35" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vírgula" xfId="20" builtinId="3" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="52">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1205,34 +1400,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <color theme="5" tint="-0.499984740745262"/>
@@ -1328,6 +1495,18 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1347,6 +1526,37 @@
         <b/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1483,14 +1693,14 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Plano de marketing" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Lista de planos" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="35"/>
-      <tableStyleElement type="headerRow" dxfId="34"/>
-      <tableStyleElement type="firstRowStripe" dxfId="33"/>
+      <tableStyleElement type="wholeTable" dxfId="51"/>
+      <tableStyleElement type="headerRow" dxfId="50"/>
+      <tableStyleElement type="firstRowStripe" dxfId="49"/>
     </tableStyle>
     <tableStyle name="Plano de marketing" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="32"/>
-      <tableStyleElement type="headerRow" dxfId="31"/>
-      <tableStyleElement type="totalRow" dxfId="30"/>
+      <tableStyleElement type="wholeTable" dxfId="48"/>
+      <tableStyleElement type="headerRow" dxfId="47"/>
+      <tableStyleElement type="totalRow" dxfId="46"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -6199,16 +6409,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Dados" displayName="Dados" ref="B6:H19" headerRowDxfId="29">
-  <autoFilter ref="B6:H19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Dados" displayName="Dados" ref="B6:H21" headerRowDxfId="45">
+  <autoFilter ref="B6:H21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa" totalsRowLabel="Total" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Status" totalsRowFunction="count" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Semana" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Responsável" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Atribuído a" dataDxfId="11" dataCellStyle="Data"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Data de início" dataDxfId="10" dataCellStyle="Data"/>
-    <tableColumn id="6" xr3:uid="{B3EC7629-E4DA-4FA6-BCF2-5E4DC4390764}" name="Data de término" dataDxfId="9" dataCellStyle="Data"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa" totalsRowLabel="Total" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Status" totalsRowFunction="count" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Semana" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Responsável" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Atribuído a" dataDxfId="40" dataCellStyle="Data"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Previsão de início" dataDxfId="39" dataCellStyle="Data"/>
+    <tableColumn id="6" xr3:uid="{B3EC7629-E4DA-4FA6-BCF2-5E4DC4390764}" name="Previsão de término" dataDxfId="38" dataCellStyle="Data"/>
   </tableColumns>
   <tableStyleInfo name="Plano de marketing" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -6220,11 +6430,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Pessoas" displayName="Pessoas" ref="B4:C11" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Pessoas" displayName="Pessoas" ref="B4:C11" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="B4:C11" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Nome" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cargo" totalsRowFunction="count" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Nome" totalsRowLabel="Total" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cargo" totalsRowFunction="count" dataDxfId="33" totalsRowDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="Lista de planos" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -6565,17 +6775,19 @@
     <tabColor theme="4" tint="0.39997558519241921"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H19"/>
+  <dimension ref="B1:H21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="64.25" style="1" customWidth="1"/>
-    <col min="3" max="7" width="17.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.25" style="1" customWidth="1"/>
+    <col min="3" max="5" width="17.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6584,19 +6796,19 @@
         <v>13</v>
       </c>
       <c r="C1" s="9"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2"/>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
       <c r="G2"/>
     </row>
     <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -6647,7 +6859,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>8</v>
@@ -6656,26 +6868,26 @@
         <v>10</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="14">
@@ -6689,18 +6901,18 @@
     </row>
     <row r="8" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="21" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="14">
@@ -6714,18 +6926,18 @@
     </row>
     <row r="9" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="21" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="14">
@@ -6739,18 +6951,20 @@
     </row>
     <row r="10" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="G10" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
         <v>45171</v>
@@ -6762,18 +6976,20 @@
     </row>
     <row r="11" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="G11" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
         <v>45171</v>
@@ -6785,170 +7001,224 @@
     </row>
     <row r="12" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="14" t="e">
-        <f t="shared" ref="G12:H18" ca="1" si="0">DATE(YEAR(TODAY())*0,0,0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H12" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
+      <c r="F12" s="21"/>
+      <c r="G12" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
+        <v>45178</v>
+      </c>
+      <c r="H12" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
+        <v>45182</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H13" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
+      <c r="F13" s="21"/>
+      <c r="G13" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
+        <v>45178</v>
+      </c>
+      <c r="H13" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
+        <v>45182</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E14" s="13"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H14" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
+      <c r="F14" s="21"/>
+      <c r="G14" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
+        <v>45178</v>
+      </c>
+      <c r="H14" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
+        <v>45182</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H15" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
+      <c r="F15" s="21"/>
+      <c r="G15" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
+        <v>45178</v>
+      </c>
+      <c r="H15" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
+        <v>45182</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H16" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
+        <v>37</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
+      </c>
+      <c r="H16" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H17" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
+      <c r="F17" s="21"/>
+      <c r="G17" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,16)</f>
+        <v>45185</v>
+      </c>
+      <c r="H17" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,20)</f>
+        <v>45189</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E18" s="13"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H18" s="14" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NUM!</v>
+      <c r="F18" s="21"/>
+      <c r="G18" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,16)</f>
+        <v>45185</v>
+      </c>
+      <c r="H18" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,20)</f>
+        <v>45189</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="27"/>
+      <c r="F19" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="G19" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
         <v>45171</v>
       </c>
       <c r="H19" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
+      </c>
+      <c r="H20" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
+      </c>
+      <c r="H21" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
         <v>45175</v>
       </c>
@@ -6958,63 +7228,117 @@
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="C2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:H19 B7:C19">
-    <cfRule type="expression" dxfId="20" priority="17">
+  <conditionalFormatting sqref="B7:C21 E12:H21 E7:H10 E11 G11:H11">
+    <cfRule type="expression" dxfId="31" priority="41">
       <formula>($C7="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:C21 E20:H21">
+    <cfRule type="expression" dxfId="30" priority="9">
+      <formula>($C20="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="10">
+      <formula>($C20="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="11">
+      <formula>($C20="Atrasado")*(clAtrasado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="12">
+      <formula>($C20="Concluído")*(clConcluído="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="13">
+      <formula>(clPersonalizado1="ATIVADO")*($C20=txtPersonalizado1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="14">
+      <formula>(clPersonalizado2="ATIVADO")*($C20=txtPersonalizado2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="15">
+      <formula>(clPersonalizado3="ATIVADO")*($C20=txtPersonalizado3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="16">
+      <formula>(clPersonalizado4="ATIVADO")*($C20=txtPersonalizado4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:D21">
+    <cfRule type="expression" dxfId="22" priority="25">
+      <formula>($C7="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="26">
       <formula>($C7="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="20" priority="27">
       <formula>($C7="Atrasado")*(clAtrasado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="28">
+    <cfRule type="expression" dxfId="19" priority="28">
       <formula>($C7="Concluído")*(clConcluído="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="30">
+    <cfRule type="expression" dxfId="18" priority="29">
       <formula>(clPersonalizado1="ATIVADO")*($C7=txtPersonalizado1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="31">
+    <cfRule type="expression" dxfId="17" priority="30">
       <formula>(clPersonalizado2="ATIVADO")*($C7=txtPersonalizado2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="32">
+    <cfRule type="expression" dxfId="16" priority="31">
       <formula>(clPersonalizado3="ATIVADO")*($C7=txtPersonalizado3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="33">
+    <cfRule type="expression" dxfId="15" priority="32">
       <formula>(clPersonalizado4="ATIVADO")*($C7=txtPersonalizado4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D19">
-    <cfRule type="expression" dxfId="8" priority="1">
-      <formula>($C7="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+  <conditionalFormatting sqref="E7:H10 B7:C21 E11 G11:H11 E12:H21">
+    <cfRule type="expression" dxfId="14" priority="45">
       <formula>($C7="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="13" priority="46">
       <formula>($C7="Atrasado")*(clAtrasado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="12" priority="52">
       <formula>($C7="Concluído")*(clConcluído="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="11" priority="54">
       <formula>(clPersonalizado1="ATIVADO")*($C7=txtPersonalizado1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="10" priority="55">
       <formula>(clPersonalizado2="ATIVADO")*($C7=txtPersonalizado2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7">
+    <cfRule type="expression" dxfId="9" priority="56">
       <formula>(clPersonalizado3="ATIVADO")*($C7=txtPersonalizado3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8">
+    <cfRule type="expression" dxfId="8" priority="57">
       <formula>(clPersonalizado4="ATIVADO")*($C7=txtPersonalizado4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>($C11="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>($C11="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>($C11="Atrasado")*(clAtrasado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>($C11="Concluído")*(clConcluído="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>(clPersonalizado1="ATIVADO")*($C11=txtPersonalizado1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>(clPersonalizado2="ATIVADO")*($C11=txtPersonalizado2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>(clPersonalizado3="ATIVADO")*($C11=txtPersonalizado3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>(clPersonalizado4="ATIVADO")*($C11=txtPersonalizado4)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="1742" yWindow="648" count="17">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Ativado ou Desativado. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" prompt="Selecione Ativado ou Desativado nesta célula para alternar o destaque da linha para o status acima. Pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C4:F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"ATIVADO,DESATIVADO"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Atribuído a na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="F7:F19" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione Atribuído a na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="F7:F21" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Nomes</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Crie um plano de projeto de Marketing nesta pasta de trabalho. Organize os dados e insira os detalhes na tabela Dados nesta planilha iniciando na célula B6. Selecione a célula B2 para navegar para a planilha Dados da lista" sqref="A1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
@@ -7030,10 +7354,10 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Atrasado está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="E3" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A categoria de status Concluído está nesta célula. Selecione Ativado ou Desativado na célula abaixo para alternar o destaque da linha para este status" sqref="F3" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="O título desta planilha está nesta célula. Selecione a célula abaixo para navegar até a planilha Dados da lista. As categorias de status estão nas células D3 a K4" sqref="B1" xr:uid="{00000000-0002-0000-0000-000015000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Nome do proprietário na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="E7:E19" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Nome do proprietário na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="E7:E21" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>Nomes</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Status na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C7:C19" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione o Status na lista. Selecione CANCELAR e pressione Alt+Seta para baixo para abrir a lista suspensa e Enter para fazer a seleção" sqref="C7:C21" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$C$3:$F$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -7071,21 +7395,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="11"/>
       <c r="C3" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:3" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -7147,7 +7471,7 @@
     <row r="11" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7402,21 +7726,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7440,14 +7764,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99945BEB-7D41-4FB6-9D32-A35A84B455C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB26FF4A-9A24-42D8-B946-9CA436224F6C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7455,4 +7771,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99945BEB-7D41-4FB6-9D32-A35A84B455C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correção das datas do plano de ação e atualização do ra
</commit_message>
<xml_diff>
--- a/Documentação/PlanoDeAção_BeCold.xlsx
+++ b/Documentação/PlanoDeAção_BeCold.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839B067E-B51D-49BA-AC80-D655DE1EADAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBAD1D4-602E-4406-9F65-27454797227D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do plano de Ação" sheetId="1" r:id="rId1"/>
@@ -6777,8 +6777,8 @@
   </sheetPr>
   <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6966,12 +6966,12 @@
         <v>17</v>
       </c>
       <c r="G10" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,2)</f>
+        <v>45201</v>
       </c>
       <c r="H10" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,6)</f>
+        <v>45205</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -6991,12 +6991,12 @@
         <v>46</v>
       </c>
       <c r="G11" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,2)</f>
+        <v>45201</v>
       </c>
       <c r="H11" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,6)</f>
+        <v>45205</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7012,12 +7012,12 @@
       <c r="E12" s="13"/>
       <c r="F12" s="21"/>
       <c r="G12" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
-        <v>45178</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,9)</f>
+        <v>45208</v>
       </c>
       <c r="H12" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
-        <v>45182</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,13)</f>
+        <v>45212</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7033,12 +7033,12 @@
       <c r="E13" s="13"/>
       <c r="F13" s="21"/>
       <c r="G13" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
-        <v>45178</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,9)</f>
+        <v>45208</v>
       </c>
       <c r="H13" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
-        <v>45182</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,13)</f>
+        <v>45212</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7054,12 +7054,12 @@
       <c r="E14" s="13"/>
       <c r="F14" s="21"/>
       <c r="G14" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
-        <v>45178</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,9)</f>
+        <v>45208</v>
       </c>
       <c r="H14" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
-        <v>45182</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,13)</f>
+        <v>45212</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7075,12 +7075,12 @@
       <c r="E15" s="13"/>
       <c r="F15" s="21"/>
       <c r="G15" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
-        <v>45178</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,9)</f>
+        <v>45208</v>
       </c>
       <c r="H15" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
-        <v>45182</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,13)</f>
+        <v>45212</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7100,12 +7100,12 @@
         <v>47</v>
       </c>
       <c r="G16" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,2)</f>
+        <v>45201</v>
       </c>
       <c r="H16" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,6)</f>
+        <v>45205</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7121,12 +7121,12 @@
       <c r="E17" s="13"/>
       <c r="F17" s="21"/>
       <c r="G17" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,16)</f>
-        <v>45185</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,16)</f>
+        <v>45215</v>
       </c>
       <c r="H17" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,20)</f>
-        <v>45189</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,20)</f>
+        <v>45219</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7142,12 +7142,12 @@
       <c r="E18" s="13"/>
       <c r="F18" s="21"/>
       <c r="G18" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,16)</f>
-        <v>45185</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,16)</f>
+        <v>45215</v>
       </c>
       <c r="H18" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,20)</f>
-        <v>45189</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,20)</f>
+        <v>45219</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -7167,12 +7167,12 @@
         <v>15</v>
       </c>
       <c r="G19" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,2)</f>
+        <v>45201</v>
       </c>
       <c r="H19" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,6)</f>
+        <v>45205</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -7192,12 +7192,12 @@
         <v>16</v>
       </c>
       <c r="G20" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,2)</f>
+        <v>45201</v>
       </c>
       <c r="H20" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,6)</f>
+        <v>45205</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -7215,12 +7215,12 @@
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,2)</f>
+        <v>45201</v>
       </c>
       <c r="H21" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,6)</f>
+        <v>45205</v>
       </c>
     </row>
   </sheetData>
@@ -7506,6 +7506,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf6cf056b5324d160236e2ac13572175">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="308e4927137fd5e63b6be1bd7725299e" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7725,25 +7743,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99945BEB-7D41-4FB6-9D32-A35A84B455C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB26FF4A-9A24-42D8-B946-9CA436224F6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ACF481C-B850-47D3-8383-E0C13159DD26}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7761,22 +7779,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB26FF4A-9A24-42D8-B946-9CA436224F6C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99945BEB-7D41-4FB6-9D32-A35A84B455C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>